<commit_message>
check a button clicking by a named range
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/Payroll.xlsx
+++ b/src/main/webapp/WEB-INF/books/Payroll.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\dev-ref\src\main\webapp\WEB-INF\book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/dev-ref/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F35D13E8-E88D-41E1-8F0F-1FD22681DF96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F45C8-B1E9-874F-931E-0D34ED7DB3E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Payroll" sheetId="2" r:id="rId1"/>
@@ -18,6 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="Department">Form!$C$5</definedName>
+    <definedName name="Generate">Payroll!$K$15</definedName>
     <definedName name="Insurance">Form!$F$11</definedName>
     <definedName name="Leave">Form!$F$10</definedName>
     <definedName name="Name">Form!$C$4</definedName>
@@ -30,18 +31,8 @@
     <definedName name="Total_Addition">Form!$C$15</definedName>
     <definedName name="Total_Deductions">Form!$F$15</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <webPublishing codePage="1252"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -723,59 +714,59 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1088,571 +1079,569 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF69E310-700E-2241-9060-6A966133B0D8}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K12"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="59" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" style="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="74" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="80" t="s">
+      <c r="D1" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="80" t="s">
+      <c r="E1" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="80" t="s">
+      <c r="F1" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="80" t="s">
+      <c r="G1" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="80" t="s">
+      <c r="H1" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="80" t="s">
+      <c r="I1" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="82" t="s">
+      <c r="K1" s="77" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+    <row r="2" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="84" t="s">
+      <c r="B2" s="79" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="80">
         <v>5000</v>
       </c>
-      <c r="D2" s="85">
+      <c r="D2" s="80">
         <f>SUM(Payroll!$C2/30/8)*8</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="E2" s="85">
+      <c r="E2" s="80">
         <f>SUM(Payroll!$C2/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F2" s="86">
+      <c r="F2" s="81">
         <f>SUM(Payroll!$C2+Payroll!$E2)</f>
         <v>5000</v>
       </c>
-      <c r="G2" s="85">
+      <c r="G2" s="80">
         <v>214</v>
       </c>
-      <c r="H2" s="85">
+      <c r="H2" s="80">
         <f>SUM(Payroll!$C2*0.06)</f>
         <v>300</v>
       </c>
-      <c r="I2" s="85">
+      <c r="I2" s="80">
         <v>54</v>
       </c>
-      <c r="J2" s="85">
+      <c r="J2" s="80">
         <f>SUM(Payroll!$D2+Payroll!$G2+Payroll!$H2-Payroll!$I2)</f>
         <v>626.66666666666663</v>
       </c>
-      <c r="K2" s="87">
+      <c r="K2" s="82">
         <f>SUM(Payroll!$F2-Payroll!$J2)</f>
         <v>4373.333333333333</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83" t="s">
+    <row r="3" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="84" t="s">
+      <c r="B3" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="85">
+      <c r="C3" s="80">
         <v>2900</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="80">
         <f>SUM(Payroll!$C3/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="80">
         <f>SUM(Payroll!$C3/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F3" s="86">
+      <c r="F3" s="81">
         <f>SUM(Payroll!$C3+Payroll!$E3)</f>
         <v>2900</v>
       </c>
-      <c r="G3" s="85">
+      <c r="G3" s="80">
         <v>102</v>
       </c>
-      <c r="H3" s="85">
+      <c r="H3" s="80">
         <f>SUM(Payroll!$C3*0)</f>
         <v>0</v>
       </c>
-      <c r="I3" s="85">
+      <c r="I3" s="80">
         <v>32.5</v>
       </c>
-      <c r="J3" s="85">
+      <c r="J3" s="80">
         <f>SUM(Payroll!$D3+Payroll!$G3+Payroll!$H3-Payroll!$I3)</f>
         <v>69.5</v>
       </c>
-      <c r="K3" s="87">
+      <c r="K3" s="82">
         <f>SUM(Payroll!$F3-Payroll!$J3)</f>
         <v>2830.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83" t="s">
+    <row r="4" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="80">
         <v>4100</v>
       </c>
-      <c r="D4" s="85">
+      <c r="D4" s="80">
         <f>SUM(Payroll!$C4/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E4" s="85">
+      <c r="E4" s="80">
         <f>SUM(Payroll!$C4/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F4" s="86">
+      <c r="F4" s="81">
         <f>SUM(Payroll!$C4+Payroll!$E4)</f>
         <v>4100</v>
       </c>
-      <c r="G4" s="85">
+      <c r="G4" s="80">
         <v>102</v>
       </c>
-      <c r="H4" s="85">
+      <c r="H4" s="80">
         <f>SUM(Payroll!$C4*0.03)</f>
         <v>123</v>
       </c>
-      <c r="I4" s="85">
+      <c r="I4" s="80">
         <v>54</v>
       </c>
-      <c r="J4" s="85">
+      <c r="J4" s="80">
         <f>SUM(Payroll!$D4+Payroll!$G4+Payroll!$H4-Payroll!$I4)</f>
         <v>171</v>
       </c>
-      <c r="K4" s="87">
+      <c r="K4" s="82">
         <f>SUM(Payroll!$F4-Payroll!$J4)</f>
         <v>3929</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83" t="s">
+    <row r="5" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="84" t="s">
+      <c r="B5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="80">
         <v>3900</v>
       </c>
-      <c r="D5" s="85">
+      <c r="D5" s="80">
         <f>-SUM(Payroll!$C5/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E5" s="85">
+      <c r="E5" s="80">
         <f>SUM(Payroll!$C5/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F5" s="86">
+      <c r="F5" s="81">
         <f>SUM(Payroll!$C5+Payroll!$E5)</f>
         <v>3900</v>
       </c>
-      <c r="G5" s="85">
+      <c r="G5" s="80">
         <v>102.4</v>
       </c>
-      <c r="H5" s="85">
+      <c r="H5" s="80">
         <f>SUM(Payroll!$C5*0.03)</f>
         <v>117</v>
       </c>
-      <c r="I5" s="85">
+      <c r="I5" s="80">
         <v>54</v>
       </c>
-      <c r="J5" s="85">
+      <c r="J5" s="80">
         <f>SUM(Payroll!$D5+Payroll!$G5+Payroll!$H5-Payroll!$I5)</f>
         <v>165.4</v>
       </c>
-      <c r="K5" s="87">
+      <c r="K5" s="82">
         <f>SUM(Payroll!$F5-Payroll!$J5)</f>
         <v>3734.6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83" t="s">
+    <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="85">
+      <c r="C6" s="80">
         <v>7800</v>
       </c>
-      <c r="D6" s="85">
+      <c r="D6" s="80">
         <f>SUM(Payroll!$C6/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E6" s="85">
+      <c r="E6" s="80">
         <f>SUM(Payroll!$C6/30/8*1.25)*4</f>
         <v>162.5</v>
       </c>
-      <c r="F6" s="86">
+      <c r="F6" s="81">
         <f>SUM(Payroll!$C6+Payroll!$E6)</f>
         <v>7962.5</v>
       </c>
-      <c r="G6" s="85">
+      <c r="G6" s="80">
         <v>214</v>
       </c>
-      <c r="H6" s="85">
+      <c r="H6" s="80">
         <f>SUM(Payroll!$C6*0.06)</f>
         <v>468</v>
       </c>
-      <c r="I6" s="85">
+      <c r="I6" s="80">
         <v>128</v>
       </c>
-      <c r="J6" s="85">
+      <c r="J6" s="80">
         <f>SUM(Payroll!$D6+Payroll!$G6+Payroll!$H6-Payroll!$I6)</f>
         <v>554</v>
       </c>
-      <c r="K6" s="87">
+      <c r="K6" s="82">
         <f>SUM(Payroll!$F6-Payroll!$J6)</f>
         <v>7408.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="83" t="s">
+    <row r="7" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="85">
+      <c r="C7" s="80">
         <v>4500</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="80">
         <f>SUM(Payroll!$C7/30/8)*4</f>
         <v>75</v>
       </c>
-      <c r="E7" s="85">
+      <c r="E7" s="80">
         <f>SUM(Payroll!$C7/30/8*1.25)*4</f>
         <v>93.75</v>
       </c>
-      <c r="F7" s="86">
+      <c r="F7" s="81">
         <f>SUM(Payroll!$C7+Payroll!$E7)</f>
         <v>4593.75</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="80">
         <v>102.4</v>
       </c>
-      <c r="H7" s="85">
+      <c r="H7" s="80">
         <f>SUM(Payroll!$C7*0)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="85">
+      <c r="I7" s="80">
         <v>54</v>
       </c>
-      <c r="J7" s="85">
+      <c r="J7" s="80">
         <f>SUM(Payroll!$D7+Payroll!$G7+Payroll!$H7-Payroll!$I7)</f>
         <v>123.4</v>
       </c>
-      <c r="K7" s="87">
+      <c r="K7" s="82">
         <f>SUM(Payroll!$F7-Payroll!$J7)</f>
         <v>4470.3500000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="83" t="s">
+    <row r="8" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="84" t="s">
+      <c r="B8" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="85">
+      <c r="C8" s="80">
         <v>5000</v>
       </c>
-      <c r="D8" s="85">
+      <c r="D8" s="80">
         <f>SUM(Payroll!$C8/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E8" s="85">
+      <c r="E8" s="80">
         <f>SUM(Payroll!$C8/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F8" s="86">
+      <c r="F8" s="81">
         <f>SUM(Payroll!$C8+Payroll!$E8)</f>
         <v>5000</v>
       </c>
-      <c r="G8" s="85">
+      <c r="G8" s="80">
         <v>102.4</v>
       </c>
-      <c r="H8" s="85">
+      <c r="H8" s="80">
         <f>SUM(Payroll!$C8*0.03)</f>
         <v>150</v>
       </c>
-      <c r="I8" s="85">
+      <c r="I8" s="80">
         <v>106</v>
       </c>
-      <c r="J8" s="85">
+      <c r="J8" s="80">
         <f>SUM(Payroll!$D8+Payroll!$G8+Payroll!$H8-Payroll!$I8)</f>
         <v>146.4</v>
       </c>
-      <c r="K8" s="87">
+      <c r="K8" s="82">
         <f>SUM(Payroll!$F8-Payroll!$J8)</f>
         <v>4853.6000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="83" t="s">
+    <row r="9" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="79" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="80">
         <v>8600</v>
       </c>
-      <c r="D9" s="85">
+      <c r="D9" s="80">
         <f>SUM(Payroll!$C9/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E9" s="85">
+      <c r="E9" s="80">
         <f>SUM(Payroll!$C9/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F9" s="86">
+      <c r="F9" s="81">
         <f>SUM(Payroll!$C9+Payroll!$E9)</f>
         <v>8600</v>
       </c>
-      <c r="G9" s="85">
+      <c r="G9" s="80">
         <v>214</v>
       </c>
-      <c r="H9" s="85">
+      <c r="H9" s="80">
         <f>SUM(Payroll!$C9*0.06)</f>
         <v>516</v>
       </c>
-      <c r="I9" s="85">
+      <c r="I9" s="80">
         <v>150</v>
       </c>
-      <c r="J9" s="85">
+      <c r="J9" s="80">
         <f>SUM(Payroll!$D9+Payroll!$G9+Payroll!$H9-Payroll!$I9)</f>
         <v>580</v>
       </c>
-      <c r="K9" s="87">
+      <c r="K9" s="82">
         <f>SUM(Payroll!$F9-Payroll!$J9)</f>
         <v>8020</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83" t="s">
+    <row r="10" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="85">
+      <c r="C10" s="80">
         <v>3200</v>
       </c>
-      <c r="D10" s="85">
+      <c r="D10" s="80">
         <f>SUM(Payroll!$C10/30/8)*16</f>
         <v>213.33333333333334</v>
       </c>
-      <c r="E10" s="85">
+      <c r="E10" s="80">
         <f>SUM(Payroll!$C10/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F10" s="86">
+      <c r="F10" s="81">
         <f>SUM(Payroll!$C10+Payroll!$E10)</f>
         <v>3200</v>
       </c>
-      <c r="G10" s="85">
+      <c r="G10" s="80">
         <v>102.4</v>
       </c>
-      <c r="H10" s="85">
+      <c r="H10" s="80">
         <f>SUM(Payroll!$C10*0)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="85">
+      <c r="I10" s="80">
         <v>32.5</v>
       </c>
-      <c r="J10" s="85">
+      <c r="J10" s="80">
         <f>SUM(Payroll!$D10+Payroll!$G10+Payroll!$H10-Payroll!$I10)</f>
         <v>283.23333333333335</v>
       </c>
-      <c r="K10" s="87">
+      <c r="K10" s="82">
         <f>SUM(Payroll!$F10-Payroll!$J10)</f>
         <v>2916.7666666666664</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="83" t="s">
+    <row r="11" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="85">
+      <c r="C11" s="80">
         <v>5000</v>
       </c>
-      <c r="D11" s="85">
+      <c r="D11" s="80">
         <f>SUM(Payroll!$C11/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E11" s="85">
+      <c r="E11" s="80">
         <f>SUM(Payroll!$C11/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F11" s="86">
+      <c r="F11" s="81">
         <f>SUM(Payroll!$C11+Payroll!$E11)</f>
         <v>5000</v>
       </c>
-      <c r="G11" s="85">
+      <c r="G11" s="80">
         <v>102.4</v>
       </c>
-      <c r="H11" s="85">
+      <c r="H11" s="80">
         <f>SUM(Payroll!$C11*0.03)</f>
         <v>150</v>
       </c>
-      <c r="I11" s="85">
+      <c r="I11" s="80">
         <v>106</v>
       </c>
-      <c r="J11" s="85">
+      <c r="J11" s="80">
         <f>SUM(Payroll!$D11+Payroll!$G11+Payroll!$H11-Payroll!$I11)</f>
         <v>146.4</v>
       </c>
-      <c r="K11" s="87">
+      <c r="K11" s="82">
         <f>SUM(Payroll!$F11-Payroll!$J11)</f>
         <v>4853.6000000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="83" t="s">
+    <row r="12" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="85">
+      <c r="C12" s="80">
         <v>8600</v>
       </c>
-      <c r="D12" s="85">
+      <c r="D12" s="80">
         <f>SUM(Payroll!$C12/30/8)*0</f>
         <v>0</v>
       </c>
-      <c r="E12" s="85">
+      <c r="E12" s="80">
         <f>SUM(Payroll!$C12/30/8*1.25)*0</f>
         <v>0</v>
       </c>
-      <c r="F12" s="86">
+      <c r="F12" s="81">
         <f>SUM(Payroll!$C12+Payroll!$E12)</f>
         <v>8600</v>
       </c>
-      <c r="G12" s="85">
+      <c r="G12" s="80">
         <v>214</v>
       </c>
-      <c r="H12" s="85">
+      <c r="H12" s="80">
         <f>SUM(Payroll!$C12*0.06)</f>
         <v>516</v>
       </c>
-      <c r="I12" s="85">
+      <c r="I12" s="80">
         <v>150</v>
       </c>
-      <c r="J12" s="85">
+      <c r="J12" s="80">
         <f>SUM(Payroll!$D12+Payroll!$G12+Payroll!$H12-Payroll!$I12)</f>
         <v>580</v>
       </c>
-      <c r="K12" s="87">
+      <c r="K12" s="82">
         <f>SUM(Payroll!$F12-Payroll!$J12)</f>
         <v>8020</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="88" t="s">
+    <row r="13" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="83" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="89"/>
-      <c r="C13" s="89">
+      <c r="B13" s="84"/>
+      <c r="C13" s="84">
         <f>SUM(Payroll!$C$2:$C$12)</f>
         <v>58600</v>
       </c>
-      <c r="D13" s="89">
+      <c r="D13" s="84">
         <f>SUM(Payroll!$D$2:$D$12)</f>
         <v>455</v>
       </c>
-      <c r="E13" s="89">
+      <c r="E13" s="84">
         <f>SUM(Payroll!$E$2:$E$12)</f>
         <v>256.25</v>
       </c>
-      <c r="F13" s="89">
+      <c r="F13" s="84">
         <f>SUM(Payroll!$F$2:$F$12)</f>
         <v>58856.25</v>
       </c>
-      <c r="G13" s="89">
+      <c r="G13" s="84">
         <f>SUM(Payroll!$G$2:$G$12)</f>
         <v>1572</v>
       </c>
-      <c r="H13" s="89">
+      <c r="H13" s="84">
         <f>SUM(Payroll!$H$2:$H$12)</f>
         <v>2340</v>
       </c>
-      <c r="I13" s="89">
+      <c r="I13" s="84">
         <f>SUBTOTAL(109,Payroll!$I$2:$I$12)</f>
         <v>921</v>
       </c>
-      <c r="J13" s="89">
+      <c r="J13" s="84">
         <f>SUBTOTAL(109,Payroll!$J$2:$J$12)</f>
         <v>3446.0000000000005</v>
       </c>
-      <c r="K13" s="90">
+      <c r="K13" s="85">
         <f>SUBTOTAL(109,Payroll!$K$2:$K$12)</f>
         <v>55410.249999999993</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="K15" s="78" t="s">
+    <row r="14" spans="1:11" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:11" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="73" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="7:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="7:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="7:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="17" spans="7:13" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="18" spans="7:13" ht="17" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="19" spans="7:13" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G19" s="67"/>
     </row>
-    <row r="20" spans="7:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:13" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="M20" s="68"/>
     </row>
-    <row r="22" spans="7:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:13" x14ac:dyDescent="0.15">
       <c r="I22" s="14"/>
       <c r="J22" s="72"/>
     </row>
-    <row r="24" spans="7:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:13" x14ac:dyDescent="0.15">
       <c r="H24" s="72"/>
     </row>
-    <row r="25" spans="7:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="7:13" x14ac:dyDescent="0.15">
       <c r="H25" s="72"/>
     </row>
   </sheetData>
@@ -1672,22 +1661,22 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="1" max="1" width="2.5" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.5" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" customWidth="1"/>
-    <col min="10" max="10" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="15.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:13" ht="51.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" ht="16" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="2" spans="2:13" ht="52" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="36" t="s">
         <v>6</v>
       </c>
@@ -1700,7 +1689,7 @@
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
     </row>
-    <row r="3" spans="2:13" s="3" customFormat="1" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" s="3" customFormat="1" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1711,7 +1700,7 @@
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="53" t="s">
         <v>1</v>
       </c>
@@ -1728,7 +1717,7 @@
       <c r="I4" s="26"/>
       <c r="J4" s="26"/>
     </row>
-    <row r="5" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="55" t="s">
         <v>7</v>
       </c>
@@ -1746,7 +1735,7 @@
       <c r="J5" s="28"/>
       <c r="M5" s="12"/>
     </row>
-    <row r="6" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="55" t="s">
         <v>2</v>
       </c>
@@ -1763,18 +1752,18 @@
       <c r="K6" s="11"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="10"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="77"/>
-      <c r="E7" s="77"/>
+      <c r="C7" s="89"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
       <c r="F7" s="1"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
       <c r="J7" s="28"/>
     </row>
-    <row r="8" spans="2:13" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" ht="25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="44" t="s">
         <v>29</v>
       </c>
@@ -1789,7 +1778,7 @@
       <c r="I8" s="10"/>
       <c r="J8" s="28"/>
     </row>
-    <row r="9" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="45"/>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
@@ -1800,7 +1789,7 @@
       <c r="I9" s="10"/>
       <c r="J9" s="28"/>
     </row>
-    <row r="10" spans="2:13" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="52" t="s">
         <v>8</v>
       </c>
@@ -1810,15 +1799,15 @@
         <v>13</v>
       </c>
       <c r="F10" s="47"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="75"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="87"/>
       <c r="K10" s="15"/>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="53" t="s">
         <v>10</v>
       </c>
@@ -1828,15 +1817,15 @@
         <v>35</v>
       </c>
       <c r="F11" s="60"/>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-      <c r="I11" s="76"/>
-      <c r="J11" s="75"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="87"/>
       <c r="K11" s="15"/>
       <c r="L11" s="15"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="56"/>
       <c r="C12" s="49"/>
       <c r="D12" s="22"/>
@@ -1852,7 +1841,7 @@
       <c r="L12" s="15"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="2:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B13" s="18"/>
       <c r="C13" s="50"/>
       <c r="D13" s="20"/>
@@ -1868,7 +1857,7 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" ht="9" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="13"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
@@ -1882,7 +1871,7 @@
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="53" t="s">
         <v>12</v>
       </c>
@@ -1900,7 +1889,7 @@
       <c r="L15" s="15"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="2:13" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" ht="10" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="13"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
@@ -1914,7 +1903,7 @@
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" ht="45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="53" t="s">
         <v>11</v>
       </c>
@@ -1932,7 +1921,7 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="13"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -1946,7 +1935,7 @@
       <c r="L18" s="15"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="13"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -1960,7 +1949,7 @@
       <c r="L19" s="15"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="13"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -1977,7 +1966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="13"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -1991,7 +1980,7 @@
       <c r="L21" s="15"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="13"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -2005,7 +1994,7 @@
       <c r="L22" s="15"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="13"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -2019,25 +2008,25 @@
       <c r="L23" s="15"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="18"/>
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="24"/>
       <c r="F24" s="65"/>
-      <c r="G24" s="73"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
       <c r="K24" s="15"/>
       <c r="L24" s="15"/>
       <c r="M24" s="15"/>
     </row>
-    <row r="25" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
+    <row r="25" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
       <c r="F25" s="65"/>
       <c r="G25" s="18"/>
       <c r="H25" s="20"/>
@@ -2047,7 +2036,7 @@
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
     </row>
-    <row r="26" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="6"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -2061,7 +2050,7 @@
       <c r="L26" s="15"/>
       <c r="M26" s="15"/>
     </row>
-    <row r="27" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="13"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -2075,7 +2064,7 @@
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="13"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -2089,7 +2078,7 @@
       <c r="L28" s="15"/>
       <c r="M28" s="15"/>
     </row>
-    <row r="29" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="13"/>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -2103,7 +2092,7 @@
       <c r="L29" s="15"/>
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="13"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -2117,7 +2106,7 @@
       <c r="L30" s="15"/>
       <c r="M30" s="15"/>
     </row>
-    <row r="31" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="13"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -2131,7 +2120,7 @@
       <c r="L31" s="15"/>
       <c r="M31" s="15"/>
     </row>
-    <row r="32" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="13"/>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -2145,21 +2134,21 @@
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
     </row>
-    <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="13"/>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
       <c r="F33" s="65"/>
-      <c r="G33" s="73"/>
-      <c r="H33" s="73"/>
-      <c r="I33" s="73"/>
-      <c r="J33" s="73"/>
+      <c r="G33" s="88"/>
+      <c r="H33" s="88"/>
+      <c r="I33" s="88"/>
+      <c r="J33" s="88"/>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
     </row>
-    <row r="34" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="6"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
@@ -2173,11 +2162,11 @@
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
     </row>
-    <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
+    <row r="35" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="88"/>
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
       <c r="F35" s="65"/>
       <c r="G35" s="13"/>
       <c r="H35" s="9"/>
@@ -2187,7 +2176,7 @@
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
     </row>
-    <row r="36" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="18"/>
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
@@ -2201,7 +2190,7 @@
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
     </row>
-    <row r="37" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="13"/>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
@@ -2215,7 +2204,7 @@
       <c r="L37" s="15"/>
       <c r="M37" s="15"/>
     </row>
-    <row r="38" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="13"/>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
@@ -2229,7 +2218,7 @@
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
     </row>
-    <row r="39" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="13"/>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
@@ -2243,21 +2232,21 @@
       <c r="L39" s="15"/>
       <c r="M39" s="15"/>
     </row>
-    <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="13"/>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="65"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="73"/>
-      <c r="I40" s="73"/>
-      <c r="J40" s="73"/>
+      <c r="G40" s="88"/>
+      <c r="H40" s="88"/>
+      <c r="I40" s="88"/>
+      <c r="J40" s="88"/>
       <c r="K40" s="15"/>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
     </row>
-    <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="18"/>
       <c r="C41" s="19"/>
       <c r="D41" s="19"/>
@@ -2271,11 +2260,11 @@
       <c r="L41" s="15"/>
       <c r="M41" s="15"/>
     </row>
-    <row r="42" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42" s="73"/>
+    <row r="42" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B42" s="88"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="88"/>
+      <c r="E42" s="88"/>
       <c r="F42" s="65"/>
       <c r="G42" s="13"/>
       <c r="H42" s="9"/>
@@ -2285,7 +2274,7 @@
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
     </row>
-    <row r="43" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="6"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -2299,7 +2288,7 @@
       <c r="L43" s="15"/>
       <c r="M43" s="15"/>
     </row>
-    <row r="44" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="13"/>
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
@@ -2313,7 +2302,7 @@
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
     </row>
-    <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="13"/>
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
@@ -2327,21 +2316,21 @@
       <c r="L45" s="15"/>
       <c r="M45" s="15"/>
     </row>
-    <row r="46" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="13"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
       <c r="E46" s="9"/>
       <c r="F46" s="65"/>
-      <c r="G46" s="73"/>
-      <c r="H46" s="73"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
+      <c r="G46" s="88"/>
+      <c r="H46" s="88"/>
+      <c r="I46" s="88"/>
+      <c r="J46" s="88"/>
       <c r="K46" s="15"/>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
     </row>
-    <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="6"/>
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
@@ -2355,11 +2344,11 @@
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
     </row>
-    <row r="48" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="73"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="73"/>
-      <c r="E48" s="73"/>
+    <row r="48" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B48" s="88"/>
+      <c r="C48" s="88"/>
+      <c r="D48" s="88"/>
+      <c r="E48" s="88"/>
       <c r="F48" s="65"/>
       <c r="G48" s="13"/>
       <c r="H48" s="9"/>
@@ -2369,7 +2358,7 @@
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
     </row>
-    <row r="49" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B49" s="18"/>
       <c r="C49" s="25"/>
       <c r="D49" s="25"/>
@@ -2383,7 +2372,7 @@
       <c r="L49" s="15"/>
       <c r="M49" s="15"/>
     </row>
-    <row r="50" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B50" s="13"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
@@ -2397,7 +2386,7 @@
       <c r="L50" s="15"/>
       <c r="M50" s="15"/>
     </row>
-    <row r="51" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B51" s="13"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
@@ -2411,21 +2400,21 @@
       <c r="L51" s="15"/>
       <c r="M51" s="15"/>
     </row>
-    <row r="52" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B52" s="13"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="9"/>
       <c r="F52" s="65"/>
-      <c r="G52" s="73"/>
-      <c r="H52" s="73"/>
-      <c r="I52" s="73"/>
-      <c r="J52" s="73"/>
+      <c r="G52" s="88"/>
+      <c r="H52" s="88"/>
+      <c r="I52" s="88"/>
+      <c r="J52" s="88"/>
       <c r="K52" s="15"/>
       <c r="L52" s="15"/>
       <c r="M52" s="15"/>
     </row>
-    <row r="53" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B53" s="13"/>
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
@@ -2439,7 +2428,7 @@
       <c r="L53" s="15"/>
       <c r="M53" s="15"/>
     </row>
-    <row r="54" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B54" s="13"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
@@ -2453,7 +2442,7 @@
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
     </row>
-    <row r="55" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B55" s="18"/>
       <c r="C55" s="19"/>
       <c r="D55" s="19"/>
@@ -2467,11 +2456,11 @@
       <c r="L55" s="15"/>
       <c r="M55" s="15"/>
     </row>
-    <row r="56" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="73"/>
-      <c r="C56" s="73"/>
-      <c r="D56" s="73"/>
-      <c r="E56" s="73"/>
+    <row r="56" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B56" s="88"/>
+      <c r="C56" s="88"/>
+      <c r="D56" s="88"/>
+      <c r="E56" s="88"/>
       <c r="F56" s="65"/>
       <c r="G56" s="13"/>
       <c r="H56" s="9"/>
@@ -2481,7 +2470,7 @@
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
     </row>
-    <row r="57" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B57" s="17"/>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
@@ -2495,7 +2484,7 @@
       <c r="L57" s="15"/>
       <c r="M57" s="15"/>
     </row>
-    <row r="58" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B58" s="13"/>
       <c r="C58" s="9"/>
       <c r="D58" s="9"/>
@@ -2509,101 +2498,101 @@
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
     </row>
-    <row r="59" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B59" s="13"/>
       <c r="C59" s="9"/>
       <c r="D59" s="9"/>
       <c r="E59" s="9"/>
       <c r="F59" s="66"/>
-      <c r="G59" s="74"/>
-      <c r="H59" s="74"/>
-      <c r="I59" s="74"/>
-      <c r="J59" s="74"/>
+      <c r="G59" s="90"/>
+      <c r="H59" s="90"/>
+      <c r="I59" s="90"/>
+      <c r="J59" s="90"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
     </row>
-    <row r="60" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="13"/>
       <c r="C60" s="9"/>
       <c r="D60" s="9"/>
       <c r="E60" s="9"/>
       <c r="F60" s="66"/>
-      <c r="G60" s="76"/>
-      <c r="H60" s="76"/>
-      <c r="I60" s="76"/>
-      <c r="J60" s="75"/>
+      <c r="G60" s="86"/>
+      <c r="H60" s="86"/>
+      <c r="I60" s="86"/>
+      <c r="J60" s="87"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
     </row>
-    <row r="61" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="13"/>
       <c r="C61" s="9"/>
       <c r="D61" s="9"/>
       <c r="E61" s="9"/>
       <c r="F61" s="66"/>
-      <c r="G61" s="76"/>
-      <c r="H61" s="76"/>
-      <c r="I61" s="76"/>
-      <c r="J61" s="75"/>
+      <c r="G61" s="86"/>
+      <c r="H61" s="86"/>
+      <c r="I61" s="86"/>
+      <c r="J61" s="87"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
     </row>
-    <row r="62" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B62" s="13"/>
       <c r="C62" s="9"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="66"/>
-      <c r="G62" s="76"/>
-      <c r="H62" s="76"/>
-      <c r="I62" s="76"/>
-      <c r="J62" s="75"/>
+      <c r="G62" s="86"/>
+      <c r="H62" s="86"/>
+      <c r="I62" s="86"/>
+      <c r="J62" s="87"/>
       <c r="K62" s="15"/>
       <c r="L62" s="15"/>
     </row>
-    <row r="63" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B63" s="13"/>
       <c r="C63" s="9"/>
       <c r="D63" s="9"/>
       <c r="E63" s="9"/>
       <c r="F63" s="66"/>
-      <c r="G63" s="76"/>
-      <c r="H63" s="76"/>
-      <c r="I63" s="76"/>
-      <c r="J63" s="75"/>
+      <c r="G63" s="86"/>
+      <c r="H63" s="86"/>
+      <c r="I63" s="86"/>
+      <c r="J63" s="87"/>
       <c r="K63" s="15"/>
       <c r="L63" s="15"/>
     </row>
-    <row r="64" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:13" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B64" s="13"/>
       <c r="C64" s="9"/>
       <c r="D64" s="9"/>
       <c r="E64" s="9"/>
       <c r="F64" s="66"/>
-      <c r="G64" s="76"/>
-      <c r="H64" s="76"/>
-      <c r="I64" s="76"/>
-      <c r="J64" s="75"/>
+      <c r="G64" s="86"/>
+      <c r="H64" s="86"/>
+      <c r="I64" s="86"/>
+      <c r="J64" s="87"/>
       <c r="K64" s="15"/>
       <c r="L64" s="15"/>
     </row>
-    <row r="65" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B65" s="17"/>
       <c r="C65" s="16"/>
       <c r="D65" s="16"/>
       <c r="E65" s="16"/>
       <c r="F65" s="66"/>
-      <c r="G65" s="76"/>
-      <c r="H65" s="76"/>
-      <c r="I65" s="76"/>
-      <c r="J65" s="75"/>
+      <c r="G65" s="86"/>
+      <c r="H65" s="86"/>
+      <c r="I65" s="86"/>
+      <c r="J65" s="87"/>
       <c r="K65" s="15"/>
       <c r="L65" s="15"/>
     </row>
-    <row r="66" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B66" s="15"/>
       <c r="C66" s="15"/>
       <c r="D66" s="15"/>
@@ -2616,7 +2605,7 @@
       <c r="K66" s="15"/>
       <c r="L66" s="15"/>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B67" s="15"/>
       <c r="C67" s="15"/>
       <c r="D67" s="15"/>
@@ -2629,7 +2618,7 @@
       <c r="K67" s="15"/>
       <c r="L67" s="15"/>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B68" s="15"/>
       <c r="C68" s="15"/>
       <c r="D68" s="15"/>
@@ -2642,7 +2631,7 @@
       <c r="K68" s="15"/>
       <c r="L68" s="15"/>
     </row>
-    <row r="69" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B69" s="15"/>
       <c r="C69" s="15"/>
       <c r="D69" s="15"/>
@@ -2655,7 +2644,7 @@
       <c r="K69" s="15"/>
       <c r="L69" s="15"/>
     </row>
-    <row r="70" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B70" s="15"/>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
@@ -2668,7 +2657,7 @@
       <c r="K70" s="15"/>
       <c r="L70" s="15"/>
     </row>
-    <row r="71" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B71" s="15"/>
       <c r="C71" s="15"/>
       <c r="D71" s="15"/>
@@ -2681,7 +2670,7 @@
       <c r="K71" s="15"/>
       <c r="L71" s="15"/>
     </row>
-    <row r="72" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B72" s="15"/>
       <c r="C72" s="15"/>
       <c r="D72" s="15"/>
@@ -2696,6 +2685,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="G59:J59"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="G64:I65"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="G62:I63"/>
+    <mergeCell ref="G60:I61"/>
+    <mergeCell ref="J60:J61"/>
     <mergeCell ref="G10:I11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="B48:E48"/>
@@ -2704,18 +2705,6 @@
     <mergeCell ref="G33:J33"/>
     <mergeCell ref="G40:J40"/>
     <mergeCell ref="G46:J46"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="G64:I65"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="G62:I63"/>
-    <mergeCell ref="G60:I61"/>
-    <mergeCell ref="J60:J61"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="G59:J59"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B42:E42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>

</xml_diff>